<commit_message>
add support for full excel export
</commit_message>
<xml_diff>
--- a/nyc_taxis/template.xlsx
+++ b/nyc_taxis/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohalpert/Desktop/opensearch-benchmark-workloads/nyc_taxis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FA1DF8-6CCC-AE41-94DF-5E945084051A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22E0BCB-4465-D547-9492-2AD07DE366AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1920" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>All results in milliseconds</t>
   </si>
@@ -74,14 +74,25 @@
   </si>
   <si>
     <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +440,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,33 +449,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -488,7 +500,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -513,7 +525,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -538,7 +550,7 @@
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -563,7 +575,7 @@
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -588,7 +600,7 @@
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -613,8 +625,8 @@
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>17</v>
+      <c r="A44" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>